<commit_message>
DB/table for Release2 created
</commit_message>
<xml_diff>
--- a/Data Dictionary_FinalProject.xlsx
+++ b/Data Dictionary_FinalProject.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cxxme\source\FinalProject\DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cxxme\source\RockPaperScissor_Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4552F3E2-BC72-4817-89CE-BBED7F3656C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADD451F-B634-4EA8-A7B0-9EBB68448D01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
   <si>
     <t>Table</t>
   </si>
@@ -70,42 +70,104 @@
 CHECK IN('PAPER','SCISSOR','ROCK')</t>
   </si>
   <si>
-    <t>DateTime</t>
-  </si>
-  <si>
-    <t>Round</t>
-  </si>
-  <si>
-    <t>COMP FK
-CHECK IN('PAPER','SCISSOR','ROCK')</t>
-  </si>
-  <si>
-    <t>COMP PK</t>
+    <t>As Above</t>
+  </si>
+  <si>
+    <t>The choices provided</t>
+  </si>
+  <si>
+    <t>The time when the game is played</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>GameID</t>
+  </si>
+  <si>
+    <t>GameResult</t>
+  </si>
+  <si>
+    <t>NumOfTurn</t>
+  </si>
+  <si>
+    <t>CHECK IN(1,3,5)</t>
+  </si>
+  <si>
+    <t>CHECK IN('W','L','D')</t>
+  </si>
+  <si>
+    <t>NAVARCHAR(1)</t>
+  </si>
+  <si>
+    <t>The result of the game</t>
+  </si>
+  <si>
+    <t>ID of the game</t>
+  </si>
+  <si>
+    <t>The time when the game is started</t>
+  </si>
+  <si>
+    <t>The choosen number of turns</t>
+  </si>
+  <si>
+    <t>Turn</t>
+  </si>
+  <si>
+    <t>TurnNumber</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>PK
+CHECK LENGTH=6</t>
+  </si>
+  <si>
+    <t>FK REF Player</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
   <si>
     <t>COMP PK
-COMP FK</t>
-  </si>
-  <si>
-    <t>As Above</t>
-  </si>
-  <si>
-    <t>The choices provided</t>
-  </si>
-  <si>
-    <t>The time when the game is played</t>
-  </si>
-  <si>
-    <t>PlayTime</t>
+COMP FK REF Game</t>
+  </si>
+  <si>
+    <t>COMP FK REF Choice</t>
+  </si>
+  <si>
+    <t>COMP PK
+CHECK IN(1,2,3,4,5)</t>
+  </si>
+  <si>
+    <t>GameStarted</t>
+  </si>
+  <si>
+    <t>TurnResult</t>
+  </si>
+  <si>
+    <t>NVARCHAR(1)</t>
+  </si>
+  <si>
+    <t>The result of the turn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -132,7 +194,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -155,79 +217,44 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,122 +535,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.81640625" customWidth="1"/>
-    <col min="3" max="3" width="19.08984375" customWidth="1"/>
-    <col min="4" max="4" width="20.26953125" customWidth="1"/>
-    <col min="5" max="5" width="30.26953125" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" customWidth="1"/>
+    <col min="2" max="2" width="26.7265625" customWidth="1"/>
+    <col min="3" max="3" width="26.90625" customWidth="1"/>
+    <col min="4" max="4" width="32.6328125" customWidth="1"/>
+    <col min="5" max="5" width="51.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:5" ht="23.5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:5" ht="23.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:5" ht="94" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="C8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="47" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="70.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="9"/>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="9"/>
+      <c r="B11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="E11" s="12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="47" x14ac:dyDescent="0.35">
+      <c r="A12" s="9"/>
+      <c r="B12" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="9"/>
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>19</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A4:A6"/>
+  <mergeCells count="2">
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A4:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>